<commit_message>
Cài đặt Laravel 8.x và copy source
</commit_message>
<xml_diff>
--- a/me-docs/31.Nang-cap-len-laravel-8.xlsx
+++ b/me-docs/31.Nang-cap-len-laravel-8.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414D6EA2-7932-4162-86A3-5CD3BD67F838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB26AFC6-3DD2-4522-9AAF-67E83FF6B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upgrading To 8.0" sheetId="1" r:id="rId1"/>
+    <sheet name="install 8.x và copy source" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Updating Dependencies</t>
   </si>
@@ -52,6 +53,120 @@
   </si>
   <si>
     <t>Check browser</t>
+  </si>
+  <si>
+    <t>composer create-project laravel/laravel:^8.0 .</t>
+  </si>
+  <si>
+    <t>Install Laravel</t>
+  </si>
+  <si>
+    <t>.env</t>
+  </si>
+  <si>
+    <t>composer require barryvdh/laravel-debugbar --dev</t>
+  </si>
+  <si>
+    <t>Install debugbar</t>
+  </si>
+  <si>
+    <t>Install laravelcollective</t>
+  </si>
+  <si>
+    <t>composer require laravelcollective/html</t>
+  </si>
+  <si>
+    <t>Copy Helpers</t>
+  </si>
+  <si>
+    <t>Copy Controller</t>
+  </si>
+  <si>
+    <t>Coppy Middleware</t>
+  </si>
+  <si>
+    <t>Copy Requests folder</t>
+  </si>
+  <si>
+    <t>Copy Model</t>
+  </si>
+  <si>
+    <t>app\User.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit User.php </t>
+  </si>
+  <si>
+    <t>Copy config\zvn.php</t>
+  </si>
+  <si>
+    <t>Copy public</t>
+  </si>
+  <si>
+    <t>Copy all file in resources\views</t>
+  </si>
+  <si>
+    <t>Copy routes\web.php</t>
+  </si>
+  <si>
+    <t>xampp\apache\conf\extra\httpd-vhosts.conf</t>
+  </si>
+  <si>
+    <t>C:\Windows\System32\drivers\etc\hosts</t>
+  </si>
+  <si>
+    <t>app\Providers\RouteServiceProvider.php</t>
+  </si>
+  <si>
+    <t>Check Laravel version</t>
+  </si>
+  <si>
+    <t>Cú pháp khai báo route của Laravel 8 khác nên sẽ phát sinh lỗi</t>
+  </si>
+  <si>
+    <t>app\Http\Kernel.php</t>
+  </si>
+  <si>
+    <t>config\filesystems.php</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Copy resources\lang\en\notify.php</t>
+  </si>
+  <si>
+    <t>edit resources\lang\en\validation.php</t>
+  </si>
+  <si>
+    <t>Using WinMerge</t>
+  </si>
+  <si>
+    <t>Copy database\migrations</t>
+  </si>
+  <si>
+    <t>Copy database\seeders</t>
+  </si>
+  <si>
+    <t>database\seeders\ArticleTableSeeder.php</t>
+  </si>
+  <si>
+    <t>database\seeders\CategoryTableSeeder.php</t>
+  </si>
+  <si>
+    <t>database\seeders\UserTableSeeder.php</t>
+  </si>
+  <si>
+    <t>database\seeders\SliderTableSeeder.php</t>
+  </si>
+  <si>
+    <t>Add namespace</t>
+  </si>
+  <si>
+    <t>Laravel 8</t>
   </si>
 </sst>
 </file>
@@ -773,6 +888,1507 @@
         <a:xfrm>
           <a:off x="609600" y="68199001"/>
           <a:ext cx="10925175" cy="5413227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>294248</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8201A6EF-A6F3-F96D-FD58-469611D22253}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="8219048" cy="6600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333029</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664D8C8A-E0B3-2CA1-A29D-BF0DD84B39D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7620000"/>
+          <a:ext cx="2771429" cy="1485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>513143</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>27905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3635F478-7761-CB0F-7A54-84145DDE425B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9715500"/>
+          <a:ext cx="9657143" cy="5361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>465524</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>189905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC2EE08-2614-AAE7-5447-02FDEAA58E79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="15621000"/>
+          <a:ext cx="9609524" cy="4761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523657</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>28310</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D797EB65-8C9B-DD46-36F1-AA423738D8BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20764500"/>
+          <a:ext cx="1742857" cy="2123810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333181</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>171286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E050EE5-6F7E-79E2-3354-1A8607E26767}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="23241000"/>
+          <a:ext cx="1552381" cy="1314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609219</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>37762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313269D6-B1AC-7E6A-065C-D52D46305B46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24955500"/>
+          <a:ext cx="3047619" cy="2704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>218743</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>9214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC94000-3B87-E587-F804-A9E88EADE448}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="28194000"/>
+          <a:ext cx="2657143" cy="2485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>599771</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>94833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E887A12-0C96-3838-8328-DE73BFEEABE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="31051500"/>
+          <a:ext cx="2428571" cy="3333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>427809</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>161667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BCEDEE9-59A2-85C1-05C4-1E6E971B54F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="35052000"/>
+          <a:ext cx="6523809" cy="2066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>503924</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>66381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E88B79-69B1-4C15-3623-9833CF273E9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="37338000"/>
+          <a:ext cx="7209524" cy="2352381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85486</xdr:colOff>
+      <xdr:row>235</xdr:row>
+      <xdr:rowOff>132929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC063EBD-A822-A013-C732-C66E1807E4AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="40195500"/>
+          <a:ext cx="1914286" cy="3371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447390</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>152000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6FAAC3-0DB8-AE04-E1B9-1B14D3E5646B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="44005500"/>
+          <a:ext cx="2276190" cy="3200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609295</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>9262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE87437F-AA5E-9137-C7BA-88999143D66C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="47625000"/>
+          <a:ext cx="2438095" cy="2104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>270</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>599771</xdr:colOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>28333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1EBFC69-F6DC-17EA-FFF7-916A9AB5C674}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="50101500"/>
+          <a:ext cx="2428571" cy="1933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>294629</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>85167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B23C23F-AA87-5322-5B9E-C313F6127ECD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="52578000"/>
+          <a:ext cx="5171429" cy="4466667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>309</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>246857</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>9286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B394C74A-2D67-2655-14D3-5B120C957E7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="57531000"/>
+          <a:ext cx="6342857" cy="1914286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>345</xdr:row>
+      <xdr:rowOff>60515</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B802C5D-85D8-C09F-C02A-C921ED1E711B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609601" y="61150500"/>
+          <a:ext cx="7248524" cy="4632515"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>608457</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>18762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A1F1EE3-D8CE-9C39-1A0A-8B35B63E6F00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="66675000"/>
+          <a:ext cx="9142857" cy="2304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>132419</xdr:colOff>
+      <xdr:row>383</xdr:row>
+      <xdr:rowOff>132976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8EC9647-14ED-534A-ECB7-7673E046A118}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="69151500"/>
+          <a:ext cx="7447619" cy="2990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323124</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>104667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A831F32-3D56-43AD-367A-7E4A06AA82D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20764500"/>
+          <a:ext cx="5809524" cy="866667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>370667</xdr:colOff>
+      <xdr:row>353</xdr:row>
+      <xdr:rowOff>47476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{769E83CB-C51A-9DE9-1CC5-74DBAB04CDA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="67818000"/>
+          <a:ext cx="6466667" cy="1190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>103784</xdr:colOff>
+      <xdr:row>338</xdr:row>
+      <xdr:rowOff>56742</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2561E706-F52E-1017-FD5C-69FD03A493BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8029575" y="61179075"/>
+          <a:ext cx="7923809" cy="3266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>386</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>589333</xdr:colOff>
+      <xdr:row>402</xdr:row>
+      <xdr:rowOff>28190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{396A4A63-EFCD-6364-58B3-DABE5A84D130}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="73533000"/>
+          <a:ext cx="9733333" cy="3076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>351619</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>123524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B410FB-8865-32F3-AC7E-7BE25BD554C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="76962000"/>
+          <a:ext cx="6447619" cy="2409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>514</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>589486</xdr:colOff>
+      <xdr:row>542</xdr:row>
+      <xdr:rowOff>180286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF732272-F3AC-B18D-F85F-506646322FA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="97917000"/>
+          <a:ext cx="8514286" cy="5514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>545</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>571</xdr:row>
+      <xdr:rowOff>80517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86AC5DC1-A4CD-EC10-4F44-22DA634258E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="103822500"/>
+          <a:ext cx="10296525" cy="5033517"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>573</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>600</xdr:row>
+      <xdr:rowOff>190109</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E729A13D-65BE-3A33-E1F4-B7B369053E36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="109156501"/>
+          <a:ext cx="10887075" cy="5333608"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>418</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590324</xdr:colOff>
+      <xdr:row>427</xdr:row>
+      <xdr:rowOff>180738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3623C96-F33F-0C39-F0FA-3E5B6C2512FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="79629000"/>
+          <a:ext cx="1809524" cy="1895238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>431</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>113143</xdr:colOff>
+      <xdr:row>462</xdr:row>
+      <xdr:rowOff>180214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7444545B-5AEC-A7F1-A98A-A997DDF6733E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="82105500"/>
+          <a:ext cx="9257143" cy="6085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>465</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>294781</xdr:colOff>
+      <xdr:row>479</xdr:row>
+      <xdr:rowOff>75857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8212FFE0-F251-4A19-A43A-502E0D7966EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="88582500"/>
+          <a:ext cx="3952381" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>481</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295010</xdr:colOff>
+      <xdr:row>488</xdr:row>
+      <xdr:rowOff>142690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2D0B695-2792-7E35-98FC-2C9B50AC0BE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="91630500"/>
+          <a:ext cx="2123810" cy="1476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>495</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>65676</xdr:colOff>
+      <xdr:row>509</xdr:row>
+      <xdr:rowOff>75857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46E04723-11D5-2887-252B-8838F59F1ED7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="94297500"/>
+          <a:ext cx="7990476" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>492</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>509</xdr:row>
+      <xdr:rowOff>184507</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B5AC829-AF46-977D-6A2C-7C2BB8B47CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144001" y="93745050"/>
+          <a:ext cx="6648450" cy="3403957"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1049,7 +2665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
+    <sheetView topLeftCell="A229" workbookViewId="0">
       <selection activeCell="C391" sqref="C391"/>
     </sheetView>
   </sheetViews>
@@ -1133,4 +2749,213 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34CCF32-D1AB-44BF-9084-F17CFC3F59CE}">
+  <dimension ref="A2:P573"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A485" workbookViewId="0">
+      <selection activeCell="N489" sqref="N489"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="321" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N321" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="481" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="491" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="492" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B492" t="s">
+        <v>41</v>
+      </c>
+      <c r="P492" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="493" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B493" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="494" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B494" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="495" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B495" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="545" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B545" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="573" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B573" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>